<commit_message>
Change files on 5/08/2024
</commit_message>
<xml_diff>
--- a/New files/Alaska Native Trival/ANTHC-23-D-426757.xlsx
+++ b/New files/Alaska Native Trival/ANTHC-23-D-426757.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAA98066-603F-475D-98E7-03A338A71077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CD0EE47-2955-423A-9E42-91EAED1DF258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{B0CCC734-F4D0-45CE-B4DA-88E3DFF057FA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E5EB2332-BFC8-40B0-9F38-4AA3A851675D}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_Summary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="59">
   <si>
     <t>Bill to</t>
   </si>
@@ -73,7 +73,7 @@
     <t>Account #4707877349</t>
   </si>
   <si>
-    <t>4055985-C1</t>
+    <t>4055985-A</t>
   </si>
   <si>
     <t>02/25/2024 - 03/09/2024</t>
@@ -118,13 +118,7 @@
     <t>Regular</t>
   </si>
   <si>
-    <t xml:space="preserve">OC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">OT </t>
-  </si>
-  <si>
-    <t>CallBack</t>
+    <t>OT</t>
   </si>
   <si>
     <t>Caregiver</t>
@@ -139,6 +133,9 @@
     <t>Sanchez, Decsy</t>
   </si>
   <si>
+    <t>OC</t>
+  </si>
+  <si>
     <t>Total Amount Due</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
   </si>
   <si>
     <t>ANTHC-23-D-426757</t>
-  </si>
-  <si>
-    <t>Surgical Services</t>
   </si>
   <si>
     <t>Aya Healthcare</t>
@@ -636,20 +630,20 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1676400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D86C51B-632D-EDD3-31E4-C84D48F19271}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F31A978-477A-0D20-0F6A-FC53E036DAA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -980,28 +974,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC4813B-76E5-484F-AFC6-04CF2509AA54}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57002FD-5D5A-4446-91F5-95959FAA7988}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="49"/>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -1014,7 +1007,7 @@
       <c r="J1" s="52"/>
       <c r="K1" s="53"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
       <c r="G2" s="7" t="s">
         <v>1</v>
@@ -1024,7 +1017,7 @@
       </c>
       <c r="K2" s="44"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="G3" s="7" t="s">
         <v>2</v>
@@ -1034,7 +1027,7 @@
       </c>
       <c r="K3" s="44"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="G4" s="7" t="s">
         <v>3</v>
@@ -1044,7 +1037,7 @@
       </c>
       <c r="K4" s="44"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="G5" s="7" t="s">
         <v>4</v>
@@ -1054,7 +1047,7 @@
       </c>
       <c r="K5" s="44"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="G6" s="7" t="s">
         <v>5</v>
@@ -1064,18 +1057,18 @@
       </c>
       <c r="K6" s="44"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="G7" s="7"/>
       <c r="J7" s="2"/>
       <c r="K7" s="44"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="J8" s="2"/>
       <c r="K8" s="44"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="G9" s="8" t="s">
         <v>6</v>
@@ -1085,14 +1078,14 @@
       </c>
       <c r="K9" s="44"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="J10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K10" s="44"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="9"/>
       <c r="J11" s="4" t="s">
@@ -1100,7 +1093,7 @@
       </c>
       <c r="K11" s="44"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="9" t="s">
         <v>0</v>
@@ -1108,7 +1101,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="44"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="9" t="s">
         <v>17</v>
@@ -1118,7 +1111,7 @@
       </c>
       <c r="K13" s="44"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="9" t="s">
         <v>18</v>
@@ -1128,7 +1121,7 @@
       </c>
       <c r="K14" s="44"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="9" t="s">
         <v>19</v>
@@ -1138,13 +1131,13 @@
       </c>
       <c r="K15" s="44"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="9"/>
       <c r="J16" s="2"/>
       <c r="K16" s="44"/>
     </row>
-    <row r="17" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="47"/>
       <c r="B17" s="1" t="s">
         <v>16</v>
@@ -1159,11 +1152,11 @@
       <c r="J17" s="1"/>
       <c r="K17" s="44"/>
     </row>
-    <row r="18" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="K18" s="44"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="10" t="s">
         <v>17</v>
@@ -1178,7 +1171,7 @@
       </c>
       <c r="K19" s="44"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -1191,11 +1184,11 @@
       </c>
       <c r="K20" s="44"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="K21" s="44"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="C22" s="26" t="s">
         <v>22</v>
@@ -1210,12 +1203,12 @@
         <v>21</v>
       </c>
       <c r="I22" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J22" s="38"/>
       <c r="K22" s="44"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="C23" s="27">
         <v>204165</v>
@@ -1235,7 +1228,7 @@
       <c r="J23" s="38"/>
       <c r="K23" s="44"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
       <c r="C24" s="28" t="s">
         <v>25</v>
@@ -1249,11 +1242,11 @@
       </c>
       <c r="K24" s="44"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="K25" s="44"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
       <c r="D26" s="26" t="s">
         <v>26</v>
@@ -1266,195 +1259,169 @@
       </c>
       <c r="K26" s="44"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
       <c r="D27" s="27" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="16">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F27" s="20">
-        <v>10200</v>
+        <v>10582.5</v>
       </c>
       <c r="K27" s="44"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
       <c r="D28" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E28" s="30">
+        <v>45</v>
+      </c>
+      <c r="F28" s="32">
+        <v>5737.52</v>
+      </c>
+      <c r="K28" s="44"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="47"/>
+      <c r="D29" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="23">
+        <v>168</v>
+      </c>
+      <c r="F29" s="25">
+        <v>16320.02</v>
+      </c>
+      <c r="K29" s="44"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="47"/>
+      <c r="K30" s="44"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="47"/>
+      <c r="D31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="44"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="47"/>
+      <c r="D32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="20">
+        <v>10</v>
+      </c>
+      <c r="G32" s="18">
         <v>105.75</v>
       </c>
-      <c r="F28" s="32">
+      <c r="H32" s="20">
         <v>1057.5</v>
       </c>
-      <c r="K28" s="44"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="47"/>
-      <c r="D29" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="16">
+      <c r="K32" s="44"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="47"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="32">
+        <v>127.5</v>
+      </c>
+      <c r="G33" s="31">
         <v>45</v>
       </c>
-      <c r="F29" s="20">
+      <c r="H33" s="32">
         <v>5737.52</v>
       </c>
-      <c r="K29" s="44"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="47"/>
-      <c r="D30" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="30">
-        <v>3</v>
-      </c>
-      <c r="F30" s="32">
-        <v>382.5</v>
-      </c>
-      <c r="K30" s="44"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="47"/>
-      <c r="D31" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="23">
-        <v>273.75</v>
-      </c>
-      <c r="F31" s="25">
-        <v>17377.52</v>
-      </c>
-      <c r="K31" s="44"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="47"/>
-      <c r="K32" s="44"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="47"/>
-      <c r="D33" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="19" t="s">
-        <v>21</v>
-      </c>
       <c r="K33" s="44"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
-      <c r="D34" s="14" t="s">
-        <v>34</v>
-      </c>
+      <c r="D34" s="14"/>
       <c r="E34" s="27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F34" s="20">
-        <v>127.5</v>
+        <v>85</v>
       </c>
       <c r="G34" s="18">
-        <v>3</v>
+        <v>120</v>
       </c>
       <c r="H34" s="20">
-        <v>382.5</v>
+        <v>10200</v>
       </c>
       <c r="K34" s="44"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
       <c r="D35" s="29"/>
       <c r="E35" s="33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F35" s="32">
-        <v>10</v>
+        <v>127.5</v>
       </c>
       <c r="G35" s="31">
-        <v>105.75</v>
+        <v>3</v>
       </c>
       <c r="H35" s="32">
-        <v>1057.5</v>
+        <v>382.5</v>
       </c>
       <c r="K35" s="44"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="47"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" s="20">
-        <v>127.5</v>
-      </c>
-      <c r="G36" s="18">
-        <v>45</v>
-      </c>
-      <c r="H36" s="20">
-        <v>5737.52</v>
+      <c r="D36" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="35"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="24">
+        <v>273.75</v>
+      </c>
+      <c r="H36" s="25">
+        <v>17377.52</v>
       </c>
       <c r="K36" s="44"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="F37" s="32">
-        <v>85</v>
-      </c>
-      <c r="G37" s="31">
-        <v>120</v>
-      </c>
-      <c r="H37" s="32">
-        <v>10200</v>
-      </c>
       <c r="K37" s="44"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="47"/>
-      <c r="D38" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="24">
-        <v>273.75</v>
-      </c>
-      <c r="H38" s="25">
-        <v>17377.52</v>
-      </c>
-      <c r="K38" s="44"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="47"/>
-      <c r="K39" s="44"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="48"/>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="46"/>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="48"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1462,18 +1429,18 @@
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D36:F36"/>
     <mergeCell ref="I22:J22"/>
     <mergeCell ref="I23:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="52" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="50" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC62594-4D86-46AC-B081-F7671C5A5D6D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C6EB49-A11D-4E10-A456-FDE788ED2B72}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1481,97 +1448,93 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="J1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="K1" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="40" t="s">
+      <c r="M1" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="N1" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="40" t="s">
+      <c r="P1" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="40" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="B2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D2" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>17</v>
@@ -1580,7 +1543,7 @@
         <v>45333</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>27</v>
@@ -1601,27 +1564,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D3" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>17</v>
@@ -1630,48 +1589,44 @@
         <v>45334</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L3" s="43">
-        <v>10.25</v>
+        <v>13</v>
       </c>
       <c r="M3" s="43">
         <v>0</v>
       </c>
       <c r="N3" s="41">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="O3" s="12">
-        <v>871.25</v>
+        <v>130</v>
       </c>
       <c r="P3" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D4" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>17</v>
@@ -1680,48 +1635,44 @@
         <v>45334</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L4" s="43">
-        <v>13</v>
+        <v>10.25</v>
       </c>
       <c r="M4" s="43">
         <v>0</v>
       </c>
       <c r="N4" s="41">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="O4" s="12">
-        <v>130</v>
+        <v>871.25</v>
       </c>
       <c r="P4" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D5" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>17</v>
@@ -1730,48 +1681,44 @@
         <v>45336</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L5" s="43">
-        <v>10.25</v>
+        <v>13</v>
       </c>
       <c r="M5" s="43">
         <v>0</v>
       </c>
       <c r="N5" s="41">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="O5" s="12">
-        <v>871.25</v>
+        <v>130</v>
       </c>
       <c r="P5" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D6" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>17</v>
@@ -1780,48 +1727,44 @@
         <v>45336</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L6" s="43">
-        <v>13</v>
+        <v>10.25</v>
       </c>
       <c r="M6" s="43">
         <v>0</v>
       </c>
       <c r="N6" s="41">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="O6" s="12">
-        <v>130</v>
+        <v>871.25</v>
       </c>
       <c r="P6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D7" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>17</v>
@@ -1830,10 +1773,10 @@
         <v>45337</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L7" s="43">
         <v>0</v>
@@ -1851,27 +1794,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D8" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>17</v>
@@ -1880,7 +1819,7 @@
         <v>45337</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>27</v>
@@ -1901,27 +1840,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D9" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>17</v>
@@ -1930,48 +1865,44 @@
         <v>45338</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L9" s="43">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M9" s="43">
-        <v>10.25</v>
+        <v>0</v>
       </c>
       <c r="N9" s="41">
-        <v>127.5</v>
+        <v>10</v>
       </c>
       <c r="O9" s="12">
-        <v>1306.8800000000001</v>
+        <v>130</v>
       </c>
       <c r="P9" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D10" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>17</v>
@@ -1980,48 +1911,44 @@
         <v>45338</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>28</v>
       </c>
       <c r="L10" s="43">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="M10" s="43">
-        <v>0</v>
+        <v>10.25</v>
       </c>
       <c r="N10" s="41">
-        <v>10</v>
+        <v>127.5</v>
       </c>
       <c r="O10" s="12">
-        <v>130</v>
+        <v>1306.8800000000001</v>
       </c>
       <c r="P10" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D11" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>17</v>
@@ -2030,10 +1957,10 @@
         <v>45339</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11" s="43">
         <v>0</v>
@@ -2051,27 +1978,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D12" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>17</v>
@@ -2080,7 +2003,7 @@
         <v>45341</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>27</v>
@@ -2101,27 +2024,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D13" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>17</v>
@@ -2130,48 +2049,44 @@
         <v>45342</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L13" s="43">
-        <v>10.25</v>
+        <v>13</v>
       </c>
       <c r="M13" s="43">
         <v>0</v>
       </c>
       <c r="N13" s="41">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="O13" s="12">
-        <v>871.25</v>
+        <v>130</v>
       </c>
       <c r="P13" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D14" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>17</v>
@@ -2180,48 +2095,44 @@
         <v>45342</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L14" s="43">
-        <v>13</v>
+        <v>10.25</v>
       </c>
       <c r="M14" s="43">
         <v>0</v>
       </c>
       <c r="N14" s="41">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="O14" s="12">
-        <v>130</v>
+        <v>871.25</v>
       </c>
       <c r="P14" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D15" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>17</v>
@@ -2230,7 +2141,7 @@
         <v>45343</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>27</v>
@@ -2251,27 +2162,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D16" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>17</v>
@@ -2280,10 +2187,10 @@
         <v>45344</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L16" s="43">
         <v>0</v>
@@ -2301,27 +2208,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D17" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>17</v>
@@ -2330,48 +2233,44 @@
         <v>45344</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L17" s="43">
-        <v>8.75</v>
+        <v>13</v>
       </c>
       <c r="M17" s="43">
         <v>0</v>
       </c>
       <c r="N17" s="41">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="O17" s="12">
-        <v>743.75</v>
+        <v>130</v>
       </c>
       <c r="P17" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D18" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>17</v>
@@ -2380,48 +2279,44 @@
         <v>45344</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L18" s="43">
-        <v>13</v>
+        <v>8.75</v>
       </c>
       <c r="M18" s="43">
         <v>0</v>
       </c>
       <c r="N18" s="41">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="O18" s="12">
-        <v>130</v>
+        <v>743.75</v>
       </c>
       <c r="P18" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D19" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>17</v>
@@ -2430,10 +2325,10 @@
         <v>45345</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L19" s="43">
         <v>0</v>
@@ -2451,27 +2346,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D20" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>17</v>
@@ -2480,13 +2371,13 @@
         <v>45354</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L20" s="43">
-        <v>10.75</v>
+        <v>13</v>
       </c>
       <c r="M20" s="43">
         <v>0</v>
@@ -2495,33 +2386,29 @@
         <v>10</v>
       </c>
       <c r="O20" s="12">
-        <v>107.5</v>
+        <v>130</v>
       </c>
       <c r="P20" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D21" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>17</v>
@@ -2530,13 +2417,13 @@
         <v>45354</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L21" s="43">
-        <v>13</v>
+        <v>10.75</v>
       </c>
       <c r="M21" s="43">
         <v>0</v>
@@ -2545,33 +2432,29 @@
         <v>10</v>
       </c>
       <c r="O21" s="12">
-        <v>130</v>
+        <v>107.5</v>
       </c>
       <c r="P21" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D22" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>17</v>
@@ -2580,7 +2463,7 @@
         <v>45355</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K22" s="12" t="s">
         <v>27</v>
@@ -2601,27 +2484,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D23" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>17</v>
@@ -2630,7 +2509,7 @@
         <v>45356</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>27</v>
@@ -2651,27 +2530,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D24" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>17</v>
@@ -2680,48 +2555,44 @@
         <v>45357</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="L24" s="43">
-        <v>10.25</v>
+        <v>13</v>
       </c>
       <c r="M24" s="43">
         <v>0</v>
       </c>
       <c r="N24" s="41">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="O24" s="12">
-        <v>871.25</v>
+        <v>130</v>
       </c>
       <c r="P24" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D25" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>17</v>
@@ -2730,48 +2601,44 @@
         <v>45357</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L25" s="43">
-        <v>13</v>
+        <v>10.25</v>
       </c>
       <c r="M25" s="43">
         <v>0</v>
       </c>
       <c r="N25" s="41">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="O25" s="12">
-        <v>130</v>
+        <v>871.25</v>
       </c>
       <c r="P25" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D26" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>17</v>
@@ -2780,48 +2647,44 @@
         <v>45358</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L26" s="43">
-        <v>9.25</v>
+        <v>0</v>
       </c>
       <c r="M26" s="43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="41">
-        <v>85</v>
+        <v>127.5</v>
       </c>
       <c r="O26" s="12">
-        <v>786.25</v>
+        <v>127.5</v>
       </c>
       <c r="P26" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D27" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>17</v>
@@ -2830,48 +2693,44 @@
         <v>45358</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L27" s="43">
-        <v>0</v>
+        <v>9.25</v>
       </c>
       <c r="M27" s="43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27" s="41">
-        <v>127.5</v>
+        <v>85</v>
       </c>
       <c r="O27" s="12">
-        <v>127.5</v>
+        <v>786.25</v>
       </c>
       <c r="P27" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D28" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>17</v>
@@ -2880,48 +2739,44 @@
         <v>45359</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="L28" s="43">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M28" s="43">
-        <v>10.25</v>
+        <v>0</v>
       </c>
       <c r="N28" s="41">
-        <v>127.5</v>
+        <v>10</v>
       </c>
       <c r="O28" s="12">
-        <v>1306.8800000000001</v>
+        <v>40</v>
       </c>
       <c r="P28" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D29" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>17</v>
@@ -2930,48 +2785,44 @@
         <v>45359</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="K29" s="12" t="s">
         <v>28</v>
       </c>
       <c r="L29" s="43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M29" s="43">
-        <v>0</v>
+        <v>10.25</v>
       </c>
       <c r="N29" s="41">
-        <v>10</v>
+        <v>127.5</v>
       </c>
       <c r="O29" s="12">
-        <v>40</v>
+        <v>1306.8800000000001</v>
       </c>
       <c r="P29" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="12">
+        <v>204165</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="12" t="s">
         <v>49</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="12">
-        <v>204165</v>
-      </c>
-      <c r="D30" s="12">
-        <v>204165</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>17</v>
@@ -2980,10 +2831,10 @@
         <v>45360</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L30" s="43">
         <v>3</v>
@@ -3003,278 +2854,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="49" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A7B740158B06348BBFDD0A82FAE521C" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b9ca6de6a992593ec3295afdb73980d5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="45be6600-ce97-4f91-b2b5-90c5c801df6a" xmlns:ns3="4ff60255-49bc-4e52-8060-8afe9711eecb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c3625fcdb5b97911e04df756c65f947" ns2:_="" ns3:_="">
-    <xsd:import namespace="45be6600-ce97-4f91-b2b5-90c5c801df6a"/>
-    <xsd:import namespace="4ff60255-49bc-4e52-8060-8afe9711eecb"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="45be6600-ce97-4f91-b2b5-90c5c801df6a" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="94b3629e-20aa-442c-aac2-3c67759175e0" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="23" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="24" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4ff60255-49bc-4e52-8060-8afe9711eecb" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{6c69ecb4-97a0-434f-9afd-668c5bcfe455}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="4ff60255-49bc-4e52-8060-8afe9711eecb">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{333A6436-3C61-4355-8FE9-D59C442D6908}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{886AED0B-53A1-4EBD-9FBD-90E07CC67520}"/>
 </file>
</xml_diff>

<commit_message>
New invoices for QA
</commit_message>
<xml_diff>
--- a/New files/Alaska Native Trival/ANTHC-23-D-426757.xlsx
+++ b/New files/Alaska Native Trival/ANTHC-23-D-426757.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EACF558-DC83-466E-8A36-C9DE0F501874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BBF21A3-47B6-4A7E-8EB7-3A289487AA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D83B1ACF-FCEA-4811-A55B-C36B789089E2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0E7115E5-9AF4-4899-83ED-BDF700D86ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_Summary" sheetId="1" r:id="rId1"/>
@@ -612,20 +612,20 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>134620</xdr:rowOff>
+      <xdr:rowOff>136525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1676400</xdr:colOff>
+      <xdr:colOff>1672590</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2961F768-0234-1938-65B7-E0D3699F9395}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{221C49B0-7E8E-1B95-BCC1-27157C6CC54F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -976,7 +976,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BD81AD-B030-49A3-9EC3-BD7D5B396BF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59063B87-FD56-41D5-8AF6-B486129CF3B8}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -992,10 +992,10 @@
     <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1458,7 +1458,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A324BE41-E6FD-4B77-88C3-37F8CF6299E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1895BC0-121A-4CEC-A39A-22D8D4550C59}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1472,16 +1472,17 @@
     <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>